<commit_message>
Updated the utterance file favour against
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesFavorAgainst.xlsx
+++ b/SOP/Utterances/phrasesFavorAgainst.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parad\OneDrive\Two Robots\Git\SOP\Utterances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\Git\Storytelling_SR\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3539592E-22DE-4559-82CC-BE3FA56DAC33}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDEE34EA-6579-47B1-8530-EE2ADA1E121A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24008" xr2:uid="{E4B8DB12-B672-4611-9817-EB9A51AE5FB6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24015" activeTab="1" xr2:uid="{E4B8DB12-B672-4611-9817-EB9A51AE5FB6}"/>
   </bookViews>
   <sheets>
-    <sheet name="phrases" sheetId="3" r:id="rId1"/>
+    <sheet name="Utterances" sheetId="3" r:id="rId1"/>
+    <sheet name="Dropdowns Content" sheetId="4" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,13 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
-  <si>
-    <t>Favor</t>
-  </si>
-  <si>
-    <t>Against</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="69">
   <si>
     <t xml:space="preserve">Esta é a melhor decisão a ser tomada. </t>
   </si>
@@ -146,12 +144,6 @@
     <t>Recomendo escolher a outra decisão.</t>
   </si>
   <si>
-    <t>FavorEN</t>
-  </si>
-  <si>
-    <t>AgainstEN</t>
-  </si>
-  <si>
     <t>This is the best decision to be taken.</t>
   </si>
   <si>
@@ -234,13 +226,49 @@
   </si>
   <si>
     <t>I advise to choose the other option.</t>
+  </si>
+  <si>
+    <t>CATEGORY</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>PT:FAVOUR</t>
+  </si>
+  <si>
+    <t>EN:FAVOUR</t>
+  </si>
+  <si>
+    <t>EN:AGAINST</t>
+  </si>
+  <si>
+    <t>PT:AGAINST</t>
+  </si>
+  <si>
+    <t>REPETITIONS</t>
+  </si>
+  <si>
+    <t>Undefined</t>
+  </si>
+  <si>
+    <t>Repetitions</t>
+  </si>
+  <si>
+    <t>OnceInASession</t>
+  </si>
+  <si>
+    <t>OnceAndForever</t>
+  </si>
+  <si>
+    <t>Categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,16 +276,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF44546A"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD6EE"/>
+        <bgColor rgb="FFBDD6EE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -265,21 +314,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF44546A"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFBDD6EE"/>
+          <bgColor rgb="FFBDD6EE"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -356,13 +464,29 @@
 </MapInfo>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Utterances"/>
+      <sheetName val="Dropdowns Content"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C6BD1A8C-990F-4699-B406-B044F8F8DCF1}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
-  <autoFilter ref="A1:C15" xr:uid="{11638E6A-CE2D-4FFB-8001-F34F4D0EAD09}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{51ABBAA3-678B-4371-94F8-061775CDF9D1}" name="Id" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{DB4AC550-EB61-4BF5-9EF3-DDACC6FACBA0}" name="Favor"/>
-    <tableColumn id="3" xr3:uid="{46F5AE16-0BFD-425C-861A-007CEB138331}" name="Against"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C6BD1A8C-990F-4699-B406-B044F8F8DCF1}" name="Table1" displayName="Table1" ref="A1:D57" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:D57" xr:uid="{11638E6A-CE2D-4FFB-8001-F34F4D0EAD09}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{51ABBAA3-678B-4371-94F8-061775CDF9D1}" name="Id" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{740F8191-BDD7-474A-A392-A27C421C223A}" name="CATEGORY" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00555465-9C0F-49E1-91F7-1634C416E0C1}" name="REPETITIONS" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{DB4AC550-EB61-4BF5-9EF3-DDACC6FACBA0}" name="TEXT"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -665,277 +789,893 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC699C3-7B7D-494D-9389-830F8CDC6B9F}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F57"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="55.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>45</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>47</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>48</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>49</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>50</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>51</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>52</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D51" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>53</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>54</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>55</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>56</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>57</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>58</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" xr:uid="{FE4CAF82-23EB-4B19-B4AB-A05468F17E4B}">
+          <x14:formula1>
+            <xm:f>'C:\Users\Marie\Desktop\SERA\Skene\Utterances\[Sueca2.xlsx]Dropdowns Content'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C57</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C08705E-E67C-4152-83FD-D98B79125A39}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.46484375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.86328125" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Audio volume reduced and phrases break fixed.
</commit_message>
<xml_diff>
--- a/SOP/Utterances/phrasesFavorAgainst.xlsx
+++ b/SOP/Utterances/phrasesFavorAgainst.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marie\Desktop\SERA\Skene\Utterances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parad\OneDrive\Two Robots\Git\SOP\Utterances\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B46CC8C2-08F5-468F-822F-BB28B94594F8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074EFC65-3FBF-41AF-9203-92D0E825758E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24015" xr2:uid="{E4B8DB12-B672-4611-9817-EB9A51AE5FB6}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="82">
   <si>
     <t>Id</t>
   </si>
@@ -270,9 +270,6 @@
     <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; I advise to choose the other option.  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(person3)&gt;&lt;break time="1s"/&gt;&lt;ANIMATE(|animation|)&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
     <t>PT:GAZE_PB</t>
   </si>
   <si>
@@ -291,13 +288,19 @@
     <t>EN:GAZE_PBPB</t>
   </si>
   <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time="1s"/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_person|)&gt;&lt;break time="1s"/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
-  </si>
-  <si>
-    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_person|)&gt;&lt;break time="1s"/&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time="1s"/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;Gaze(|animation_side|)&gt;&lt;Gaze(|animation_person|)&gt;&lt;break time='1s'/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;Gaze(|animation_side|)&gt;&lt;Gaze(|animation_person|)&gt;&lt;break time='1s'/&gt; &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;Gaze(|animation_side|)&gt;&lt;Gaze(|animation_person|)&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time='1s'/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(|animation_person|)&gt;&lt;Gaze(|animation_side|)&gt;&lt;break time='1s'/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
+  </si>
+  <si>
+    <t>&lt;prosody pitch='|pitch|'&gt;&lt;prosody rate='|rate|'&gt;&lt;prosody volume='|volume|'&gt; &lt;Gaze(person3)&gt;&lt;ANIMATE(|animation|)&gt;&lt;break time='1s'/&gt;  &lt;/prosody&gt;&lt;/prosody&gt;&lt;/prosody&gt;</t>
   </si>
 </sst>
 </file>
@@ -841,19 +844,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC699C3-7B7D-494D-9389-830F8CDC6B9F}">
   <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="235.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1328125" customWidth="1"/>
+    <col min="4" max="4" width="235.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -869,7 +872,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -883,7 +886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -897,7 +900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -911,7 +914,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -925,7 +928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -939,7 +942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -953,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -967,7 +970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -981,7 +984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -995,7 +998,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1121,7 +1124,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1135,7 +1138,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1191,7 +1194,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1205,7 +1208,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1275,7 +1278,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1289,7 +1292,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1303,7 +1306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -1317,7 +1320,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>35</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>36</v>
       </c>
@@ -1359,7 +1362,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -1387,7 +1390,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>40</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1429,7 +1432,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>42</v>
       </c>
@@ -1443,7 +1446,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -1471,7 +1474,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -1485,7 +1488,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>47</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>48</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>49</v>
       </c>
@@ -1527,7 +1530,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>50</v>
       </c>
@@ -1541,7 +1544,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>51</v>
       </c>
@@ -1555,7 +1558,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>52</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>53</v>
       </c>
@@ -1583,7 +1586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>54</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>55</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>56</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>57</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>58</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>59</v>
       </c>
@@ -1664,10 +1667,10 @@
         <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>60</v>
       </c>
@@ -1678,91 +1681,91 @@
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>61</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>62</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>63</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>64</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>65</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>66</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1794,13 +1797,13 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -1808,7 +1811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
@@ -1816,7 +1819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -1832,55 +1835,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B10" s="8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" s="8"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" s="12"/>
     </row>
   </sheetData>

</xml_diff>